<commit_message>
added elite crew to gunnergrades file; reran modeling and grades_comp output
</commit_message>
<xml_diff>
--- a/gunnergrades.xlsx
+++ b/gunnergrades.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rgian\Dropbox\pixel starships\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krissy\Desktop\PSS\PPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775E2B84-D0E5-4BAE-99F8-9BCF9B0F4DEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31582F4A-BC05-432C-888E-069117CDB9D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9075" yWindow="2115" windowWidth="16455" windowHeight="13260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="18735" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="269">
   <si>
     <t>Admiral Serena</t>
   </si>
@@ -348,472 +348,490 @@
     <t>Messiah</t>
   </si>
   <si>
+    <t>Mistycball</t>
+  </si>
+  <si>
+    <t>Monkey King</t>
+  </si>
+  <si>
+    <t>Mousey</t>
+  </si>
+  <si>
+    <t>Mr Cray</t>
+  </si>
+  <si>
+    <t>Mr Horse</t>
+  </si>
+  <si>
+    <t>Mr Old</t>
+  </si>
+  <si>
+    <t>Mr She</t>
+  </si>
+  <si>
+    <t>Mummy</t>
+  </si>
+  <si>
+    <t>Ophiuchus</t>
+  </si>
+  <si>
+    <t>P.A.N.D.A</t>
+  </si>
+  <si>
+    <t>Ponytail Alien</t>
+  </si>
+  <si>
+    <t>Qtarian Healer</t>
+  </si>
+  <si>
+    <t>Red Ninja</t>
+  </si>
+  <si>
+    <t>Ribi</t>
+  </si>
+  <si>
+    <t>Robot</t>
+  </si>
+  <si>
+    <t>Robyna Hoots</t>
+  </si>
+  <si>
+    <t>Saint Patrick</t>
+  </si>
+  <si>
+    <t>Sakura</t>
+  </si>
+  <si>
+    <t>Scorpio</t>
+  </si>
+  <si>
+    <t>Server Eric</t>
+  </si>
+  <si>
+    <t>Sie</t>
+  </si>
+  <si>
+    <t>Squid</t>
+  </si>
+  <si>
+    <t>Teddy</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Tiffany</t>
+  </si>
+  <si>
+    <t>Tin Man</t>
+  </si>
+  <si>
+    <t>Tin Robot</t>
+  </si>
+  <si>
+    <t>Tripod</t>
+  </si>
+  <si>
+    <t>Turkey Man</t>
+  </si>
+  <si>
+    <t>Verunus</t>
+  </si>
+  <si>
+    <t>Visiri Alchemist</t>
+  </si>
+  <si>
+    <t>Vivien</t>
+  </si>
+  <si>
+    <t>Walking Skeleton</t>
+  </si>
+  <si>
+    <t>Whaler</t>
+  </si>
+  <si>
+    <t>Assassin alien</t>
+  </si>
+  <si>
+    <t>Bad Uncle</t>
+  </si>
+  <si>
+    <t>Blingy Captain</t>
+  </si>
+  <si>
+    <t>Buns</t>
+  </si>
+  <si>
+    <t>Cathulu</t>
+  </si>
+  <si>
+    <t>D.R.A.G.O.N</t>
+  </si>
+  <si>
+    <t>D.R.A.K.E</t>
+  </si>
+  <si>
+    <t>Dennis</t>
+  </si>
+  <si>
+    <t>Dr Mew</t>
+  </si>
+  <si>
+    <t>Dr Sera</t>
+  </si>
+  <si>
+    <t>Easter Bunny</t>
+  </si>
+  <si>
+    <t>Emily</t>
+  </si>
+  <si>
+    <t>Fed Medic</t>
+  </si>
+  <si>
+    <t>First Mate</t>
+  </si>
+  <si>
+    <t>Foxy Girl</t>
+  </si>
+  <si>
+    <t>Franky</t>
+  </si>
+  <si>
+    <t>Gemini</t>
+  </si>
+  <si>
+    <t>Golden Boy</t>
+  </si>
+  <si>
+    <t>Good student</t>
+  </si>
+  <si>
+    <t>Gray Virtuoso</t>
+  </si>
+  <si>
+    <t>Green Ranger - Oliver</t>
+  </si>
+  <si>
+    <t>Jessica</t>
+  </si>
+  <si>
+    <t>Jesus</t>
+  </si>
+  <si>
+    <t>Kingpin</t>
+  </si>
+  <si>
+    <t>KS Gray</t>
+  </si>
+  <si>
+    <t>Leo</t>
+  </si>
+  <si>
+    <t>Libra</t>
+  </si>
+  <si>
+    <t>Male Nurse</t>
+  </si>
+  <si>
+    <t>Mama</t>
+  </si>
+  <si>
+    <t>Masky Lia</t>
+  </si>
+  <si>
+    <t>Miss Jane</t>
+  </si>
+  <si>
+    <t>Mr Blue</t>
+  </si>
+  <si>
+    <t>Mr Egggg</t>
+  </si>
+  <si>
+    <t>Nolan</t>
+  </si>
+  <si>
+    <t>Office Exec</t>
+  </si>
+  <si>
+    <t>Omar</t>
+  </si>
+  <si>
+    <t>Paul</t>
+  </si>
+  <si>
+    <t>Professor</t>
+  </si>
+  <si>
+    <t>Reaper</t>
+  </si>
+  <si>
+    <t>Robo Santa</t>
+  </si>
+  <si>
+    <t>Salon Customer</t>
+  </si>
+  <si>
+    <t>Schrodinger</t>
+  </si>
+  <si>
+    <t>Serge Eric</t>
+  </si>
+  <si>
+    <t>Simon</t>
+  </si>
+  <si>
+    <t>Snow Joe</t>
+  </si>
+  <si>
+    <t>Soda Delivery Guy</t>
+  </si>
+  <si>
+    <t>Arctic Pole Boy</t>
+  </si>
+  <si>
+    <t>Ardent Starhuntress</t>
+  </si>
+  <si>
+    <t>Area51 Alien</t>
+  </si>
+  <si>
+    <t>Astronaut</t>
+  </si>
+  <si>
+    <t>Bad Vlad</t>
+  </si>
+  <si>
+    <t>Barot</t>
+  </si>
+  <si>
+    <t>Bio Android</t>
+  </si>
+  <si>
+    <t>Boarder Droid I</t>
+  </si>
+  <si>
+    <t>Boarder Droid II</t>
+  </si>
+  <si>
+    <t>Boarder Droid III</t>
+  </si>
+  <si>
+    <t>Boarder Droid IV</t>
+  </si>
+  <si>
+    <t>Boarder Droid V</t>
+  </si>
+  <si>
+    <t>Bobby</t>
+  </si>
+  <si>
+    <t>Cancer</t>
+  </si>
+  <si>
+    <t>Captain Mack Swallow</t>
+  </si>
+  <si>
+    <t>Cat Boy</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Defender Droid I</t>
+  </si>
+  <si>
+    <t>Defender Droid II</t>
+  </si>
+  <si>
+    <t>Defender Droid III</t>
+  </si>
+  <si>
+    <t>Defender Droid IV</t>
+  </si>
+  <si>
+    <t>Defender Droid V</t>
+  </si>
+  <si>
+    <t>Demon Boy</t>
+  </si>
+  <si>
+    <t>Dracorpse</t>
+  </si>
+  <si>
+    <t>Edward</t>
+  </si>
+  <si>
+    <t>Engineer Bob</t>
+  </si>
+  <si>
+    <t>Fed Bobby</t>
+  </si>
+  <si>
+    <t>Fed Laura</t>
+  </si>
+  <si>
+    <t>Fed Lisa</t>
+  </si>
+  <si>
+    <t>Fed Michelle</t>
+  </si>
+  <si>
+    <t>Fed Peter</t>
+  </si>
+  <si>
+    <t>Fed Tony</t>
+  </si>
+  <si>
+    <t>Helen</t>
+  </si>
+  <si>
+    <t>Henry</t>
+  </si>
+  <si>
+    <t>King Ellie</t>
+  </si>
+  <si>
+    <t>Laura</t>
+  </si>
+  <si>
+    <t>Lisa</t>
+  </si>
+  <si>
+    <t>Mini Droid I</t>
+  </si>
+  <si>
+    <t>Mini Droid II</t>
+  </si>
+  <si>
+    <t>Mini Droid III</t>
+  </si>
+  <si>
+    <t>Old Driver</t>
+  </si>
+  <si>
+    <t>Pinkzilla</t>
+  </si>
+  <si>
+    <t>Pirate Alex</t>
+  </si>
+  <si>
+    <t>Pirate Edward</t>
+  </si>
+  <si>
+    <t>Pirate Lia</t>
+  </si>
+  <si>
+    <t>Pirate Loretta</t>
+  </si>
+  <si>
+    <t>Pirate Michelle</t>
+  </si>
+  <si>
+    <t>Pirate Tony</t>
+  </si>
+  <si>
+    <t>Qtarian Bobby</t>
+  </si>
+  <si>
+    <t>Qtarian Edward</t>
+  </si>
+  <si>
+    <t>Qtarian Laura</t>
+  </si>
+  <si>
+    <t>Qtarian Lisa</t>
+  </si>
+  <si>
+    <t>Qtarian Michelle</t>
+  </si>
+  <si>
+    <t>Qtarian Tony</t>
+  </si>
+  <si>
+    <t>Roach</t>
+  </si>
+  <si>
+    <t>Rocky</t>
+  </si>
+  <si>
+    <t>Service Droid I</t>
+  </si>
+  <si>
+    <t>Service Droid II</t>
+  </si>
+  <si>
+    <t>Service Droid III</t>
+  </si>
+  <si>
+    <t>Service Droid IV</t>
+  </si>
+  <si>
+    <t>Service Droid V</t>
+  </si>
+  <si>
+    <t>Sphinx</t>
+  </si>
+  <si>
+    <t>Stevo</t>
+  </si>
+  <si>
+    <t>Stove Tops</t>
+  </si>
+  <si>
+    <t>Tony</t>
+  </si>
+  <si>
+    <t>Transport Driver</t>
+  </si>
+  <si>
+    <t>Zombie</t>
+  </si>
+  <si>
+    <t>Zombieee</t>
+  </si>
+  <si>
+    <t>Gunner</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>CrewName</t>
+  </si>
+  <si>
+    <t>Big Football Fan</t>
+  </si>
+  <si>
+    <t>Mikael Monnier</t>
+  </si>
+  <si>
+    <t>Oren Marcus</t>
+  </si>
+  <si>
+    <t>Rob</t>
+  </si>
+  <si>
+    <t>Kent</t>
+  </si>
+  <si>
+    <t>Monk</t>
+  </si>
+  <si>
     <t>Michelle</t>
-  </si>
-  <si>
-    <t>Mistycball</t>
-  </si>
-  <si>
-    <t>Monkey King</t>
-  </si>
-  <si>
-    <t>Mousey</t>
-  </si>
-  <si>
-    <t>Mr Cray</t>
-  </si>
-  <si>
-    <t>Mr Horse</t>
-  </si>
-  <si>
-    <t>Mr Old</t>
-  </si>
-  <si>
-    <t>Mr She</t>
-  </si>
-  <si>
-    <t>Mummy</t>
-  </si>
-  <si>
-    <t>Ophiuchus</t>
-  </si>
-  <si>
-    <t>P.A.N.D.A</t>
-  </si>
-  <si>
-    <t>Ponytail Alien</t>
-  </si>
-  <si>
-    <t>Qtarian Healer</t>
-  </si>
-  <si>
-    <t>Red Ninja</t>
-  </si>
-  <si>
-    <t>Ribi</t>
-  </si>
-  <si>
-    <t>Robot</t>
-  </si>
-  <si>
-    <t>Robyna Hoots</t>
-  </si>
-  <si>
-    <t>Saint Patrick</t>
-  </si>
-  <si>
-    <t>Sakura</t>
-  </si>
-  <si>
-    <t>Scorpio</t>
-  </si>
-  <si>
-    <t>Server Eric</t>
-  </si>
-  <si>
-    <t>Sie</t>
-  </si>
-  <si>
-    <t>Squid</t>
-  </si>
-  <si>
-    <t>Teddy</t>
-  </si>
-  <si>
-    <t>Thomas</t>
-  </si>
-  <si>
-    <t>Tiffany</t>
-  </si>
-  <si>
-    <t>Tin Man</t>
-  </si>
-  <si>
-    <t>Tin Robot</t>
-  </si>
-  <si>
-    <t>Tripod</t>
-  </si>
-  <si>
-    <t>Turkey Man</t>
-  </si>
-  <si>
-    <t>Verunus</t>
-  </si>
-  <si>
-    <t>Visiri Alchemist</t>
-  </si>
-  <si>
-    <t>Vivien</t>
-  </si>
-  <si>
-    <t>Walking Skeleton</t>
-  </si>
-  <si>
-    <t>Whaler</t>
-  </si>
-  <si>
-    <t>Assassin alien</t>
-  </si>
-  <si>
-    <t>Bad Uncle</t>
-  </si>
-  <si>
-    <t>Blingy Captain</t>
-  </si>
-  <si>
-    <t>Buns</t>
-  </si>
-  <si>
-    <t>Cathulu</t>
-  </si>
-  <si>
-    <t>D.R.A.G.O.N</t>
-  </si>
-  <si>
-    <t>D.R.A.K.E</t>
-  </si>
-  <si>
-    <t>Dennis</t>
-  </si>
-  <si>
-    <t>Dr Mew</t>
-  </si>
-  <si>
-    <t>Dr Sera</t>
-  </si>
-  <si>
-    <t>Easter Bunny</t>
-  </si>
-  <si>
-    <t>Emily</t>
-  </si>
-  <si>
-    <t>Fed Medic</t>
-  </si>
-  <si>
-    <t>First Mate</t>
-  </si>
-  <si>
-    <t>Foxy Girl</t>
-  </si>
-  <si>
-    <t>Franky</t>
-  </si>
-  <si>
-    <t>Gemini</t>
-  </si>
-  <si>
-    <t>Golden Boy</t>
-  </si>
-  <si>
-    <t>Good student</t>
-  </si>
-  <si>
-    <t>Gray Virtuoso</t>
-  </si>
-  <si>
-    <t>Green Ranger - Oliver</t>
-  </si>
-  <si>
-    <t>Jessica</t>
-  </si>
-  <si>
-    <t>Jesus</t>
-  </si>
-  <si>
-    <t>Kingpin</t>
-  </si>
-  <si>
-    <t>KS Gray</t>
-  </si>
-  <si>
-    <t>Leo</t>
-  </si>
-  <si>
-    <t>Libra</t>
-  </si>
-  <si>
-    <t>Male Nurse</t>
-  </si>
-  <si>
-    <t>Mama</t>
-  </si>
-  <si>
-    <t>Masky Lia</t>
-  </si>
-  <si>
-    <t>Miss Jane</t>
-  </si>
-  <si>
-    <t>Mr Blue</t>
-  </si>
-  <si>
-    <t>Mr Egggg</t>
-  </si>
-  <si>
-    <t>Nolan</t>
-  </si>
-  <si>
-    <t>Office Exec</t>
-  </si>
-  <si>
-    <t>Omar</t>
-  </si>
-  <si>
-    <t>Paul</t>
-  </si>
-  <si>
-    <t>Professor</t>
-  </si>
-  <si>
-    <t>Reaper</t>
-  </si>
-  <si>
-    <t>Robo Santa</t>
-  </si>
-  <si>
-    <t>Salon Customer</t>
-  </si>
-  <si>
-    <t>Schrodinger</t>
-  </si>
-  <si>
-    <t>Serge Eric</t>
-  </si>
-  <si>
-    <t>Simon</t>
-  </si>
-  <si>
-    <t>Snow Joe</t>
-  </si>
-  <si>
-    <t>Soda Delivery Guy</t>
-  </si>
-  <si>
-    <t>Arctic Pole Boy</t>
-  </si>
-  <si>
-    <t>Ardent Starhuntress</t>
-  </si>
-  <si>
-    <t>Area51 Alien</t>
-  </si>
-  <si>
-    <t>Astronaut</t>
-  </si>
-  <si>
-    <t>Bad Vlad</t>
-  </si>
-  <si>
-    <t>Barot</t>
-  </si>
-  <si>
-    <t>Bio Android</t>
-  </si>
-  <si>
-    <t>Boarder Droid I</t>
-  </si>
-  <si>
-    <t>Boarder Droid II</t>
-  </si>
-  <si>
-    <t>Boarder Droid III</t>
-  </si>
-  <si>
-    <t>Boarder Droid IV</t>
-  </si>
-  <si>
-    <t>Boarder Droid V</t>
-  </si>
-  <si>
-    <t>Bobby</t>
-  </si>
-  <si>
-    <t>Cancer</t>
-  </si>
-  <si>
-    <t>Captain Mack Swallow</t>
-  </si>
-  <si>
-    <t>Cat Boy</t>
-  </si>
-  <si>
-    <t>David</t>
-  </si>
-  <si>
-    <t>Defender Droid I</t>
-  </si>
-  <si>
-    <t>Defender Droid II</t>
-  </si>
-  <si>
-    <t>Defender Droid III</t>
-  </si>
-  <si>
-    <t>Defender Droid IV</t>
-  </si>
-  <si>
-    <t>Defender Droid V</t>
-  </si>
-  <si>
-    <t>Demon Boy</t>
-  </si>
-  <si>
-    <t>Dracorpse</t>
-  </si>
-  <si>
-    <t>Edward</t>
-  </si>
-  <si>
-    <t>Engineer Bob</t>
-  </si>
-  <si>
-    <t>Fed Bobby</t>
-  </si>
-  <si>
-    <t>Fed Laura</t>
-  </si>
-  <si>
-    <t>Fed Lisa</t>
-  </si>
-  <si>
-    <t>Fed Michelle</t>
-  </si>
-  <si>
-    <t>Fed Peter</t>
-  </si>
-  <si>
-    <t>Fed Tony</t>
-  </si>
-  <si>
-    <t>Helen</t>
-  </si>
-  <si>
-    <t>Henry</t>
-  </si>
-  <si>
-    <t>King Ellie</t>
-  </si>
-  <si>
-    <t>Laura</t>
-  </si>
-  <si>
-    <t>Lisa</t>
-  </si>
-  <si>
-    <t>Mini Droid I</t>
-  </si>
-  <si>
-    <t>Mini Droid II</t>
-  </si>
-  <si>
-    <t>Mini Droid III</t>
-  </si>
-  <si>
-    <t>Old Driver</t>
-  </si>
-  <si>
-    <t>Pinkzilla</t>
-  </si>
-  <si>
-    <t>Pirate Alex</t>
-  </si>
-  <si>
-    <t>Pirate Edward</t>
-  </si>
-  <si>
-    <t>Pirate Lia</t>
-  </si>
-  <si>
-    <t>Pirate Loretta</t>
-  </si>
-  <si>
-    <t>Pirate Michelle</t>
-  </si>
-  <si>
-    <t>Pirate Tony</t>
-  </si>
-  <si>
-    <t>Qtarian Bobby</t>
-  </si>
-  <si>
-    <t>Qtarian Edward</t>
-  </si>
-  <si>
-    <t>Qtarian Laura</t>
-  </si>
-  <si>
-    <t>Qtarian Lisa</t>
-  </si>
-  <si>
-    <t>Qtarian Michelle</t>
-  </si>
-  <si>
-    <t>Qtarian Tony</t>
-  </si>
-  <si>
-    <t>Roach</t>
-  </si>
-  <si>
-    <t>Rocky</t>
-  </si>
-  <si>
-    <t>Service Droid I</t>
-  </si>
-  <si>
-    <t>Service Droid II</t>
-  </si>
-  <si>
-    <t>Service Droid III</t>
-  </si>
-  <si>
-    <t>Service Droid IV</t>
-  </si>
-  <si>
-    <t>Service Droid V</t>
-  </si>
-  <si>
-    <t>Sphinx</t>
-  </si>
-  <si>
-    <t>Stevo</t>
-  </si>
-  <si>
-    <t>Stove Tops</t>
-  </si>
-  <si>
-    <t>Tony</t>
-  </si>
-  <si>
-    <t>Transport Driver</t>
-  </si>
-  <si>
-    <t>Zombie</t>
-  </si>
-  <si>
-    <t>Zombieee</t>
-  </si>
-  <si>
-    <t>Gunner</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>CrewName</t>
   </si>
 </sst>
 </file>
@@ -1160,10 +1178,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B257"/>
+  <dimension ref="A1:B263"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A110" sqref="A110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1173,10 +1191,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1184,7 +1202,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1192,7 +1210,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1200,7 +1218,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1208,7 +1226,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1216,7 +1234,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1224,7 +1242,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1232,7 +1250,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1240,7 +1258,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1248,7 +1266,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1256,7 +1274,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1264,7 +1282,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1272,7 +1290,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1280,7 +1298,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1288,7 +1306,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1296,7 +1314,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1304,7 +1322,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1312,7 +1330,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1320,7 +1338,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1328,7 +1346,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1336,7 +1354,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1344,7 +1362,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1352,7 +1370,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1360,7 +1378,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1368,7 +1386,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1376,7 +1394,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1384,7 +1402,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -1392,7 +1410,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1400,7 +1418,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1408,7 +1426,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1416,7 +1434,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1424,7 +1442,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1432,7 +1450,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1440,7 +1458,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1448,7 +1466,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1456,7 +1474,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1464,7 +1482,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1472,7 +1490,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1480,7 +1498,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1488,7 +1506,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1496,7 +1514,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -1504,7 +1522,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1512,7 +1530,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -1520,7 +1538,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -1528,7 +1546,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -1536,7 +1554,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1544,7 +1562,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1552,7 +1570,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -1560,7 +1578,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -1568,7 +1586,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1576,7 +1594,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -1584,7 +1602,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -1592,7 +1610,7 @@
         <v>51</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -1600,7 +1618,7 @@
         <v>52</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -1608,7 +1626,7 @@
         <v>53</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -1616,7 +1634,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1624,7 +1642,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1632,7 +1650,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -1640,7 +1658,7 @@
         <v>57</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -1648,7 +1666,7 @@
         <v>58</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -1656,7 +1674,7 @@
         <v>59</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -1664,7 +1682,7 @@
         <v>60</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -1672,7 +1690,7 @@
         <v>61</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -1680,7 +1698,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -1688,7 +1706,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -1696,7 +1714,7 @@
         <v>64</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -1704,7 +1722,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -1712,7 +1730,7 @@
         <v>66</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -1720,7 +1738,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -1728,7 +1746,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -1736,7 +1754,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -1744,7 +1762,7 @@
         <v>70</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -1752,7 +1770,7 @@
         <v>71</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -1760,7 +1778,7 @@
         <v>72</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -1768,7 +1786,7 @@
         <v>73</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -1776,7 +1794,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -1784,7 +1802,7 @@
         <v>75</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -1792,7 +1810,7 @@
         <v>76</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -1800,7 +1818,7 @@
         <v>77</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -1808,7 +1826,7 @@
         <v>78</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -1816,7 +1834,7 @@
         <v>79</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -1824,7 +1842,7 @@
         <v>80</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -1832,7 +1850,7 @@
         <v>81</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -1840,7 +1858,7 @@
         <v>82</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -1848,7 +1866,7 @@
         <v>83</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -1856,7 +1874,7 @@
         <v>84</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -1864,7 +1882,7 @@
         <v>85</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -1872,7 +1890,7 @@
         <v>86</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -1880,7 +1898,7 @@
         <v>87</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -1888,7 +1906,7 @@
         <v>88</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -1896,7 +1914,7 @@
         <v>89</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -1904,7 +1922,7 @@
         <v>90</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -1912,7 +1930,7 @@
         <v>91</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -1920,7 +1938,7 @@
         <v>92</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -1928,7 +1946,7 @@
         <v>93</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -1936,7 +1954,7 @@
         <v>94</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -1944,7 +1962,7 @@
         <v>95</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -1952,7 +1970,7 @@
         <v>96</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -1960,7 +1978,7 @@
         <v>97</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -1968,7 +1986,7 @@
         <v>98</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -1976,7 +1994,7 @@
         <v>99</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -1984,7 +2002,7 @@
         <v>100</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -1992,7 +2010,7 @@
         <v>101</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -2000,7 +2018,7 @@
         <v>102</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -2008,7 +2026,7 @@
         <v>103</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -2016,7 +2034,7 @@
         <v>104</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -2024,7 +2042,7 @@
         <v>105</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -2032,1199 +2050,1247 @@
         <v>106</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>107</v>
+        <v>268</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B150" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B158" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B161" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B165" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B166" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B167" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B168" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B169" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B170" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B171" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B172" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B173" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B174" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B175" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B176" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B177" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B178" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B179" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B180" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B181" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B182" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B183" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B184" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B185" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B186" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B187" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B188" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B189" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B190" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B191" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B192" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B193" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B194" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B195" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B196" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B197" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B198" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B199" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B200" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B201" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B202" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B203" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B204" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B205" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B206" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B207" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B208" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B209" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B210" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B211" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B212" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B213" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B214" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B215" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B216" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B217" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B218" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B219" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B220" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B221" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B222" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B223" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B224" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B225" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B226" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B227" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B229" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B230" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B231" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B232" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B233" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B234" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B235" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B236" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B237" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B238" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B239" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B240" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B241" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B242" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B243" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B244" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B245" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B246" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B247" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B248" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B249" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B250" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B251" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B252" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B253" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B254" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B255" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B256" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B257" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A258" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B258" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A259" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B259" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A260" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B260" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A261" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B261" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A262" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B262" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A263" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B263" s="1" t="s">
+        <v>260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>